<commit_message>
aspirantes completos del 7 de agosto de 2024
</commit_message>
<xml_diff>
--- a/Agosto/05 agosto/montaña/PLANTILLA LISTA DE ASPIRANTES EVALUATEC 2024 ITS MONTAÑA.xlsx
+++ b/Agosto/05 agosto/montaña/PLANTILLA LISTA DE ASPIRANTES EVALUATEC 2024 ITS MONTAÑA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\05 agosto\montaña\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxoC\OneDrive\Documents\EVALUATEC2024\Agosto\05 agosto\montaña\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B84091-D8FD-48AD-9020-DAFE479026D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF142A9D-8617-40A1-825C-B984A82C710D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUATEC" sheetId="1" r:id="rId1"/>
@@ -3162,20 +3162,20 @@
   <dimension ref="A1:M271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A39"/>
+      <selection sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="40" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="47.625" customWidth="1"/>
+    <col min="5" max="5" width="16" style="1" customWidth="1"/>
     <col min="6" max="6" width="43.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.375" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="23.875" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="23.875" style="4" customWidth="1"/>
     <col min="10" max="10" width="21.375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.375" style="4" customWidth="1"/>

</xml_diff>